<commit_message>
"Next to final submission" for the MS-NEO dApp competition
</commit_message>
<xml_diff>
--- a/neo-npcc/NPC.dApps.NeoDraw.Main/Unknown_cs-Release.xlsx
+++ b/neo-npcc/NPC.dApps.NeoDraw.Main/Unknown_cs-Release.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
   <si>
     <t>Tally by Opcode</t>
   </si>
@@ -39,6 +39,9 @@
     <t>0x04</t>
   </si>
   <si>
+    <t>0x05</t>
+  </si>
+  <si>
     <t>0x06</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>0x0B</t>
   </si>
   <si>
+    <t>0x0C</t>
+  </si>
+  <si>
     <t>0x0D</t>
   </si>
   <si>
@@ -60,15 +66,24 @@
     <t>0x0F</t>
   </si>
   <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
     <t>0x13</t>
   </si>
   <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
     <t>0x16</t>
   </si>
   <si>
-    <t>0x17</t>
-  </si>
-  <si>
     <t>0x18</t>
   </si>
   <si>
@@ -84,7 +99,7 @@
     <t>0x1E</t>
   </si>
   <si>
-    <t>0x21</t>
+    <t>0x28</t>
   </si>
   <si>
     <t>0x4F</t>
@@ -126,9 +141,18 @@
     <t>0x5C</t>
   </si>
   <si>
+    <t>0x5D</t>
+  </si>
+  <si>
     <t>0x5E</t>
   </si>
   <si>
+    <t>0x5F</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
     <t>0x61</t>
   </si>
   <si>
@@ -189,9 +213,6 @@
     <t>0x9E</t>
   </si>
   <si>
-    <t>0x9F</t>
-  </si>
-  <si>
     <t>0xC0</t>
   </si>
   <si>
@@ -207,6 +228,9 @@
     <t>0xC5</t>
   </si>
   <si>
+    <t>0xFF</t>
+  </si>
+  <si>
     <t>Opcode &gt;</t>
   </si>
   <si>
@@ -255,9 +279,18 @@
     <t>PUSH12</t>
   </si>
   <si>
+    <t>PUSH13</t>
+  </si>
+  <si>
     <t>PUSH14</t>
   </si>
   <si>
+    <t>PUSH15</t>
+  </si>
+  <si>
+    <t>PUSH16</t>
+  </si>
+  <si>
     <t>NOP</t>
   </si>
   <si>
@@ -318,9 +351,6 @@
     <t>NUMNOTEQUAL</t>
   </si>
   <si>
-    <t>LT</t>
-  </si>
-  <si>
     <t>ARRAYSIZE</t>
   </si>
   <si>
@@ -334,6 +364,9 @@
   </si>
   <si>
     <t>NEWARRAY</t>
+  </si>
+  <si>
+    <t>_STORAGE</t>
   </si>
   <si>
     <t>Cost &gt;</t>
@@ -888,27 +921,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1229,24 +1242,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BK18"/>
+  <dimension ref="A2:BS18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="A8:XFD8"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="44" max="44" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.5546875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -1430,16 +1439,40 @@
       <c r="BK4" t="s">
         <v>61</v>
       </c>
+      <c r="BL4" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1448,177 +1481,201 @@
         <v>4</v>
       </c>
       <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
         <v>6</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>9</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>11</v>
       </c>
-      <c r="L5">
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
         <v>13</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>14</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>15</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
+        <v>17</v>
+      </c>
+      <c r="R5">
+        <v>18</v>
+      </c>
+      <c r="S5">
         <v>19</v>
       </c>
-      <c r="P5">
+      <c r="T5">
+        <v>20</v>
+      </c>
+      <c r="U5">
+        <v>21</v>
+      </c>
+      <c r="V5">
         <v>22</v>
       </c>
-      <c r="Q5">
-        <v>23</v>
-      </c>
-      <c r="R5">
+      <c r="W5">
         <v>24</v>
       </c>
-      <c r="S5">
+      <c r="X5">
         <v>25</v>
       </c>
-      <c r="T5">
+      <c r="Y5">
         <v>27</v>
       </c>
-      <c r="U5">
+      <c r="Z5">
         <v>28</v>
       </c>
-      <c r="V5">
+      <c r="AA5">
         <v>30</v>
       </c>
-      <c r="W5">
-        <v>33</v>
-      </c>
-      <c r="X5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>69</v>
+      <c r="AB5">
+        <v>40</v>
       </c>
       <c r="AC5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AD5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AE5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AF5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AG5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AI5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AJ5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AK5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AL5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AM5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AN5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AO5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AP5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AQ5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AR5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AS5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AT5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AU5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AV5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AW5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AX5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AY5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AZ5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="BA5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="BB5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="BC5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="BD5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="BE5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="BF5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="BG5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="BH5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="BI5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="BJ5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="BK5" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>110</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>112</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>114</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1726,28 +1783,28 @@
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AN6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AO6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AP6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AQ6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AR6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AS6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AT6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AU6">
         <v>1E-3</v>
@@ -1800,67 +1857,91 @@
       <c r="BK6">
         <v>1E-3</v>
       </c>
+      <c r="BL6">
+        <v>1E-3</v>
+      </c>
+      <c r="BM6">
+        <v>1E-3</v>
+      </c>
+      <c r="BN6">
+        <v>1E-3</v>
+      </c>
+      <c r="BO6">
+        <v>1E-3</v>
+      </c>
+      <c r="BP6">
+        <v>1E-3</v>
+      </c>
+      <c r="BQ6">
+        <v>1E-3</v>
+      </c>
+      <c r="BR6">
+        <v>1E-3</v>
+      </c>
+      <c r="BS6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D7">
-        <v>848</v>
+        <v>668</v>
       </c>
       <c r="E7">
-        <v>885</v>
+        <v>471</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>3</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
       </c>
       <c r="K7">
         <v>3</v>
       </c>
       <c r="L7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="N7">
-        <v>19</v>
-      </c>
-      <c r="O7">
-        <v>4</v>
-      </c>
-      <c r="P7">
-        <v>4</v>
-      </c>
-      <c r="Q7">
-        <v>2</v>
-      </c>
-      <c r="R7">
-        <v>47</v>
-      </c>
       <c r="S7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <v>1</v>
@@ -1869,183 +1950,207 @@
         <v>3</v>
       </c>
       <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>18</v>
+      </c>
+      <c r="Y7">
+        <v>2</v>
+      </c>
+      <c r="Z7">
         <v>1</v>
       </c>
-      <c r="X7">
+      <c r="AA7">
+        <v>13</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>655</v>
+      </c>
+      <c r="AE7">
+        <v>835</v>
+      </c>
+      <c r="AF7">
+        <v>449</v>
+      </c>
+      <c r="AG7">
+        <v>126</v>
+      </c>
+      <c r="AH7">
+        <v>120</v>
+      </c>
+      <c r="AI7">
+        <v>74</v>
+      </c>
+      <c r="AJ7">
+        <v>105</v>
+      </c>
+      <c r="AK7">
+        <v>48</v>
+      </c>
+      <c r="AL7">
+        <v>45</v>
+      </c>
+      <c r="AM7">
+        <v>24</v>
+      </c>
+      <c r="AN7">
+        <v>19</v>
+      </c>
+      <c r="AO7">
+        <v>4</v>
+      </c>
+      <c r="AP7">
+        <v>5</v>
+      </c>
+      <c r="AQ7">
         <v>2</v>
       </c>
-      <c r="Y7">
-        <v>864</v>
-      </c>
-      <c r="Z7">
-        <v>1186</v>
-      </c>
-      <c r="AA7">
-        <v>756</v>
-      </c>
-      <c r="AB7">
-        <v>208</v>
-      </c>
-      <c r="AC7">
-        <v>204</v>
-      </c>
-      <c r="AD7">
-        <v>125</v>
-      </c>
-      <c r="AE7">
-        <v>191</v>
-      </c>
-      <c r="AF7">
-        <v>83</v>
-      </c>
-      <c r="AG7">
-        <v>77</v>
-      </c>
-      <c r="AH7">
-        <v>38</v>
-      </c>
-      <c r="AI7">
-        <v>33</v>
-      </c>
-      <c r="AJ7">
-        <v>2</v>
-      </c>
-      <c r="AK7">
+      <c r="AR7">
+        <v>9</v>
+      </c>
+      <c r="AS7">
+        <v>3</v>
+      </c>
+      <c r="AT7">
+        <v>1059</v>
+      </c>
+      <c r="AU7">
+        <v>186</v>
+      </c>
+      <c r="AV7">
+        <v>7</v>
+      </c>
+      <c r="AW7">
+        <v>14</v>
+      </c>
+      <c r="AX7">
+        <v>185</v>
+      </c>
+      <c r="AY7">
+        <v>94</v>
+      </c>
+      <c r="AZ7">
+        <v>1608</v>
+      </c>
+      <c r="BA7">
+        <v>1608</v>
+      </c>
+      <c r="BB7">
+        <v>36</v>
+      </c>
+      <c r="BC7">
+        <v>202</v>
+      </c>
+      <c r="BD7">
+        <v>1811</v>
+      </c>
+      <c r="BE7">
+        <v>12</v>
+      </c>
+      <c r="BF7">
+        <v>470</v>
+      </c>
+      <c r="BG7">
+        <v>137</v>
+      </c>
+      <c r="BH7">
+        <v>660</v>
+      </c>
+      <c r="BI7">
+        <v>3</v>
+      </c>
+      <c r="BJ7">
+        <v>6</v>
+      </c>
+      <c r="BK7">
+        <v>1</v>
+      </c>
+      <c r="BL7">
+        <v>10</v>
+      </c>
+      <c r="BM7">
+        <v>3</v>
+      </c>
+      <c r="BN7">
+        <v>4</v>
+      </c>
+      <c r="BO7">
+        <v>1</v>
+      </c>
+      <c r="BP7">
+        <v>1316</v>
+      </c>
+      <c r="BQ7">
+        <v>918</v>
+      </c>
+      <c r="BR7">
+        <v>279</v>
+      </c>
+      <c r="BS7">
         <v>5</v>
       </c>
-      <c r="AL7">
-        <v>1639</v>
-      </c>
-      <c r="AM7">
-        <v>247</v>
-      </c>
-      <c r="AN7">
-        <v>25</v>
-      </c>
-      <c r="AO7">
-        <v>19</v>
-      </c>
-      <c r="AP7">
-        <v>244</v>
-      </c>
-      <c r="AQ7">
-        <v>31</v>
-      </c>
-      <c r="AR7">
-        <v>2302</v>
-      </c>
-      <c r="AS7">
-        <v>2302</v>
-      </c>
-      <c r="AT7">
-        <v>49</v>
-      </c>
-      <c r="AU7">
-        <v>260</v>
-      </c>
-      <c r="AV7">
-        <v>2575</v>
-      </c>
-      <c r="AW7">
-        <v>8</v>
-      </c>
-      <c r="AX7">
-        <v>701</v>
-      </c>
-      <c r="AY7">
-        <v>190</v>
-      </c>
-      <c r="AZ7">
-        <v>1265</v>
-      </c>
-      <c r="BA7">
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8">
+        <v>668</v>
+      </c>
+      <c r="E8">
+        <v>471</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="BB7">
-        <v>16</v>
-      </c>
-      <c r="BC7">
-        <v>4</v>
-      </c>
-      <c r="BD7">
-        <v>21</v>
-      </c>
-      <c r="BE7">
-        <v>8</v>
-      </c>
-      <c r="BF7">
-        <v>4</v>
-      </c>
-      <c r="BG7">
-        <v>10</v>
-      </c>
-      <c r="BH7">
-        <v>1</v>
-      </c>
-      <c r="BI7">
-        <v>1937</v>
-      </c>
-      <c r="BJ7">
-        <v>1296</v>
-      </c>
-      <c r="BK7">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8">
-        <v>848</v>
-      </c>
-      <c r="E8">
-        <v>885</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
       <c r="G8">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
       <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
         <v>3</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
       </c>
       <c r="K8">
         <v>3</v>
       </c>
       <c r="L8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
         <v>4</v>
       </c>
-      <c r="N8">
-        <v>19</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8">
-        <v>4</v>
-      </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8">
-        <v>47</v>
-      </c>
       <c r="S8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <v>1</v>
@@ -2054,143 +2159,167 @@
         <v>3</v>
       </c>
       <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>18</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+      <c r="Z8">
         <v>1</v>
       </c>
-      <c r="X8">
+      <c r="AA8">
+        <v>13</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>655</v>
+      </c>
+      <c r="AE8">
+        <v>835</v>
+      </c>
+      <c r="AF8">
+        <v>449</v>
+      </c>
+      <c r="AG8">
+        <v>126</v>
+      </c>
+      <c r="AH8">
+        <v>120</v>
+      </c>
+      <c r="AI8">
+        <v>74</v>
+      </c>
+      <c r="AJ8">
+        <v>105</v>
+      </c>
+      <c r="AK8">
+        <v>48</v>
+      </c>
+      <c r="AL8">
+        <v>45</v>
+      </c>
+      <c r="AM8">
+        <v>24</v>
+      </c>
+      <c r="AN8">
+        <v>19</v>
+      </c>
+      <c r="AO8">
+        <v>4</v>
+      </c>
+      <c r="AP8">
+        <v>5</v>
+      </c>
+      <c r="AQ8">
         <v>2</v>
       </c>
-      <c r="Y8">
-        <v>864</v>
-      </c>
-      <c r="Z8">
-        <v>1186</v>
-      </c>
-      <c r="AA8">
-        <v>756</v>
-      </c>
-      <c r="AB8">
-        <v>208</v>
-      </c>
-      <c r="AC8">
-        <v>204</v>
-      </c>
-      <c r="AD8">
-        <v>125</v>
-      </c>
-      <c r="AE8">
-        <v>191</v>
-      </c>
-      <c r="AF8">
-        <v>83</v>
-      </c>
-      <c r="AG8">
-        <v>77</v>
-      </c>
-      <c r="AH8">
-        <v>38</v>
-      </c>
-      <c r="AI8">
-        <v>33</v>
-      </c>
-      <c r="AJ8">
-        <v>2</v>
-      </c>
-      <c r="AK8">
+      <c r="AR8">
+        <v>9</v>
+      </c>
+      <c r="AS8">
+        <v>3</v>
+      </c>
+      <c r="AT8">
+        <v>1059</v>
+      </c>
+      <c r="AU8">
+        <v>186</v>
+      </c>
+      <c r="AV8">
+        <v>7</v>
+      </c>
+      <c r="AW8">
+        <v>14</v>
+      </c>
+      <c r="AX8">
+        <v>185</v>
+      </c>
+      <c r="AY8">
+        <v>94</v>
+      </c>
+      <c r="AZ8">
+        <v>1608</v>
+      </c>
+      <c r="BA8">
+        <v>1608</v>
+      </c>
+      <c r="BB8">
+        <v>36</v>
+      </c>
+      <c r="BC8">
+        <v>202</v>
+      </c>
+      <c r="BD8">
+        <v>1811</v>
+      </c>
+      <c r="BE8">
+        <v>12</v>
+      </c>
+      <c r="BF8">
+        <v>470</v>
+      </c>
+      <c r="BG8">
+        <v>137</v>
+      </c>
+      <c r="BH8">
+        <v>660</v>
+      </c>
+      <c r="BI8">
+        <v>3</v>
+      </c>
+      <c r="BJ8">
+        <v>6</v>
+      </c>
+      <c r="BK8">
+        <v>1</v>
+      </c>
+      <c r="BL8">
+        <v>10</v>
+      </c>
+      <c r="BM8">
+        <v>3</v>
+      </c>
+      <c r="BN8">
+        <v>4</v>
+      </c>
+      <c r="BO8">
+        <v>1</v>
+      </c>
+      <c r="BP8">
+        <v>1316</v>
+      </c>
+      <c r="BQ8">
+        <v>918</v>
+      </c>
+      <c r="BR8">
+        <v>279</v>
+      </c>
+      <c r="BS8">
         <v>5</v>
       </c>
-      <c r="AL8">
-        <v>1639</v>
-      </c>
-      <c r="AM8">
-        <v>247</v>
-      </c>
-      <c r="AN8">
-        <v>25</v>
-      </c>
-      <c r="AO8">
-        <v>19</v>
-      </c>
-      <c r="AP8">
-        <v>244</v>
-      </c>
-      <c r="AQ8">
-        <v>31</v>
-      </c>
-      <c r="AR8">
-        <v>2302</v>
-      </c>
-      <c r="AS8">
-        <v>2302</v>
-      </c>
-      <c r="AT8">
-        <v>49</v>
-      </c>
-      <c r="AU8">
-        <v>260</v>
-      </c>
-      <c r="AV8">
-        <v>2575</v>
-      </c>
-      <c r="AW8">
-        <v>8</v>
-      </c>
-      <c r="AX8">
-        <v>701</v>
-      </c>
-      <c r="AY8">
-        <v>190</v>
-      </c>
-      <c r="AZ8">
-        <v>1265</v>
-      </c>
-      <c r="BA8">
-        <v>3</v>
-      </c>
-      <c r="BB8">
-        <v>16</v>
-      </c>
-      <c r="BC8">
-        <v>4</v>
-      </c>
-      <c r="BD8">
-        <v>21</v>
-      </c>
-      <c r="BE8">
-        <v>8</v>
-      </c>
-      <c r="BF8">
-        <v>4</v>
-      </c>
-      <c r="BG8">
-        <v>10</v>
-      </c>
-      <c r="BH8">
-        <v>1</v>
-      </c>
-      <c r="BI8">
-        <v>1937</v>
-      </c>
-      <c r="BJ8">
-        <v>1296</v>
-      </c>
-      <c r="BK8">
-        <v>351</v>
-      </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D9">
-        <v>21145</v>
+        <v>14400</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>1</v>
       </c>
@@ -2374,16 +2503,40 @@
       <c r="BK13" t="s">
         <v>61</v>
       </c>
+      <c r="BL13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN13" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO13" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>67</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>68</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -2392,177 +2545,201 @@
         <v>4</v>
       </c>
       <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
         <v>6</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>9</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>10</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>11</v>
       </c>
-      <c r="L14">
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
         <v>13</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>14</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>15</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
+        <v>17</v>
+      </c>
+      <c r="R14">
+        <v>18</v>
+      </c>
+      <c r="S14">
         <v>19</v>
       </c>
-      <c r="P14">
+      <c r="T14">
+        <v>20</v>
+      </c>
+      <c r="U14">
+        <v>21</v>
+      </c>
+      <c r="V14">
         <v>22</v>
       </c>
-      <c r="Q14">
-        <v>23</v>
-      </c>
-      <c r="R14">
+      <c r="W14">
         <v>24</v>
       </c>
-      <c r="S14">
+      <c r="X14">
         <v>25</v>
       </c>
-      <c r="T14">
+      <c r="Y14">
         <v>27</v>
       </c>
-      <c r="U14">
+      <c r="Z14">
         <v>28</v>
       </c>
-      <c r="V14">
+      <c r="AA14">
         <v>30</v>
       </c>
-      <c r="W14">
-        <v>33</v>
-      </c>
-      <c r="X14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>69</v>
+      <c r="AB14">
+        <v>40</v>
       </c>
       <c r="AC14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AD14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AE14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AF14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AG14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AI14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AJ14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AK14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AL14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AM14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AN14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AO14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AP14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AQ14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AR14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AS14" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AT14" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AU14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AV14" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AW14" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AX14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AY14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AZ14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="BA14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="BB14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="BC14" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="BD14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="BE14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="BF14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="BG14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="BH14" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="BI14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="BJ14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="BK14" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>109</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>110</v>
+      </c>
+      <c r="BO14" t="s">
+        <v>111</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>112</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>113</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>114</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2670,28 +2847,28 @@
         <v>0</v>
       </c>
       <c r="AM15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AN15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AO15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AP15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AQ15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AR15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AS15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AT15">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="AU15">
         <v>1E-3</v>
@@ -2744,16 +2921,40 @@
       <c r="BK15">
         <v>1E-3</v>
       </c>
+      <c r="BL15">
+        <v>1E-3</v>
+      </c>
+      <c r="BM15">
+        <v>1E-3</v>
+      </c>
+      <c r="BN15">
+        <v>1E-3</v>
+      </c>
+      <c r="BO15">
+        <v>1E-3</v>
+      </c>
+      <c r="BP15">
+        <v>1E-3</v>
+      </c>
+      <c r="BQ15">
+        <v>1E-3</v>
+      </c>
+      <c r="BR15">
+        <v>1E-3</v>
+      </c>
+      <c r="BS15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2861,279 +3062,324 @@
         <v>0</v>
       </c>
       <c r="AM16">
-        <v>0.247</v>
+        <v>0</v>
       </c>
       <c r="AN16">
-        <v>2.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="AO16">
-        <v>1.9E-2</v>
+        <v>0</v>
       </c>
       <c r="AP16">
-        <v>0.24399999999999999</v>
+        <v>0</v>
       </c>
       <c r="AQ16">
-        <v>3.1E-2</v>
+        <v>0</v>
       </c>
       <c r="AR16">
-        <v>2.302</v>
+        <v>0</v>
       </c>
       <c r="AS16">
-        <v>2.302</v>
+        <v>0</v>
       </c>
       <c r="AT16">
-        <v>4.9000000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="AU16">
-        <v>0.26</v>
+        <v>0.186</v>
       </c>
       <c r="AV16">
-        <v>2.5750000000000002</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AW16">
-        <v>8.0000000000000002E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AX16">
-        <v>0.70099999999999996</v>
+        <v>0.185</v>
       </c>
       <c r="AY16">
-        <v>0.19</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AZ16">
-        <v>1.2649999999999999</v>
+        <v>1.6080000000000001</v>
       </c>
       <c r="BA16">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="BB16">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="BC16">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="BD16">
+        <v>1.8109999999999999</v>
+      </c>
+      <c r="BE16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="BF16">
+        <v>0.47</v>
+      </c>
+      <c r="BG16">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="BH16">
+        <v>0.66</v>
+      </c>
+      <c r="BI16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="BB16">
-        <v>1.6E-2</v>
-      </c>
-      <c r="BC16">
+      <c r="BJ16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="BL16">
+        <v>0.01</v>
+      </c>
+      <c r="BM16">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BN16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="BD16">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="BE16">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="BF16">
+      <c r="BO16">
+        <v>0</v>
+      </c>
+      <c r="BP16">
+        <v>1.3160000000000001</v>
+      </c>
+      <c r="BQ16">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="BR16">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="BS16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:71" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AU17">
+        <v>0.186</v>
+      </c>
+      <c r="AV17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AW17">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AX17">
+        <v>0.185</v>
+      </c>
+      <c r="AY17">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AZ17">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="BA17">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="BB17">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="BC17">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="BD17">
+        <v>1.8109999999999999</v>
+      </c>
+      <c r="BE17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="BF17">
+        <v>0.47</v>
+      </c>
+      <c r="BG17">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="BH17">
+        <v>0.66</v>
+      </c>
+      <c r="BI17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BJ17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="BK17">
+        <v>0</v>
+      </c>
+      <c r="BL17">
+        <v>0.01</v>
+      </c>
+      <c r="BM17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BN17">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="BG16">
-        <v>0.01</v>
-      </c>
-      <c r="BH16">
-        <v>0</v>
-      </c>
-      <c r="BI16">
-        <v>1.9370000000000001</v>
-      </c>
-      <c r="BJ16">
-        <v>1.296</v>
-      </c>
-      <c r="BK16">
-        <v>0.35099999999999998</v>
+      <c r="BO17">
+        <v>0</v>
+      </c>
+      <c r="BP17">
+        <v>1.3160000000000001</v>
+      </c>
+      <c r="BQ17">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="BR17">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="BS17">
+        <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:63" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17">
-        <v>0</v>
-      </c>
-      <c r="AD17">
-        <v>0</v>
-      </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17">
-        <v>0</v>
-      </c>
-      <c r="AH17">
-        <v>0</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
-      </c>
-      <c r="AJ17">
-        <v>0</v>
-      </c>
-      <c r="AK17">
-        <v>0</v>
-      </c>
-      <c r="AL17">
-        <v>0</v>
-      </c>
-      <c r="AM17">
-        <v>0.247</v>
-      </c>
-      <c r="AN17">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AO17">
-        <v>1.9E-2</v>
-      </c>
-      <c r="AP17">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="AQ17">
-        <v>3.1E-2</v>
-      </c>
-      <c r="AR17">
-        <v>2.302</v>
-      </c>
-      <c r="AS17">
-        <v>2.302</v>
-      </c>
-      <c r="AT17">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="AU17">
-        <v>0.26</v>
-      </c>
-      <c r="AV17">
-        <v>2.5750000000000002</v>
-      </c>
-      <c r="AW17">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="AX17">
-        <v>0.70099999999999996</v>
-      </c>
-      <c r="AY17">
-        <v>0.19</v>
-      </c>
-      <c r="AZ17">
-        <v>1.2649999999999999</v>
-      </c>
-      <c r="BA17">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="BB17">
-        <v>1.6E-2</v>
-      </c>
-      <c r="BC17">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="BD17">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="BE17">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="BF17">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="BG17">
-        <v>0.01</v>
-      </c>
-      <c r="BH17">
-        <v>0</v>
-      </c>
-      <c r="BI17">
-        <v>1.9370000000000001</v>
-      </c>
-      <c r="BJ17">
-        <v>1.296</v>
-      </c>
-      <c r="BK17">
-        <v>0.35099999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="3:63" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:71" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D18">
-        <v>13.868</v>
+        <v>14.569000000000001</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A17:XFD17">
-    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:XFD8">
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>